<commit_message>
the evaluation section in report is modified
</commit_message>
<xml_diff>
--- a/report/evaluations/wrk_results/evaluation_summary_21-08-14.xlsx
+++ b/report/evaluations/wrk_results/evaluation_summary_21-08-14.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26840" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="520" yWindow="0" windowWidth="38660" windowHeight="26500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="wrk data" sheetId="1" r:id="rId1"/>
     <sheet name="ab data" sheetId="2" r:id="rId2"/>
     <sheet name="Saturation Test" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="73">
   <si>
     <t>30 sec</t>
   </si>
@@ -219,6 +220,27 @@
   </si>
   <si>
     <t>Percentage</t>
+  </si>
+  <si>
+    <t>CouchBase</t>
+  </si>
+  <si>
+    <t>WordPress</t>
+  </si>
+  <si>
+    <t>1hr</t>
+  </si>
+  <si>
+    <t>10hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Proxy</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -507,7 +529,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -609,8 +631,84 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,6 +798,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -733,17 +840,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="177">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -794,6 +900,44 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -844,6 +988,44 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -895,7 +1077,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1145,11 +1326,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2059584600"/>
-        <c:axId val="2104525688"/>
+        <c:axId val="-2145921928"/>
+        <c:axId val="-2145914808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2059584600"/>
+        <c:axId val="-2145921928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1211,7 +1392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2104525688"/>
+        <c:crossAx val="-2145914808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1219,7 +1400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2104525688"/>
+        <c:axId val="-2145914808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="305.0"/>
@@ -1284,14 +1465,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2059584600"/>
+        <c:crossAx val="-2145921928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1366,7 +1546,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1630,11 +1809,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114744520"/>
-        <c:axId val="-2114738568"/>
+        <c:axId val="-2145842424"/>
+        <c:axId val="-2145836472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114744520"/>
+        <c:axId val="-2145842424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1691,7 +1870,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114738568"/>
+        <c:crossAx val="-2145836472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1699,7 +1878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114738568"/>
+        <c:axId val="-2145836472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="258.0"/>
@@ -1767,7 +1946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114744520"/>
+        <c:crossAx val="-2145842424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="0.2"/>
@@ -1775,7 +1954,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2007,11 +2185,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2050896360"/>
-        <c:axId val="-2050894952"/>
+        <c:axId val="-2145790184"/>
+        <c:axId val="-2145787112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2050896360"/>
+        <c:axId val="-2145790184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2021,7 +2199,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2050894952"/>
+        <c:crossAx val="-2145787112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2029,7 +2207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2050894952"/>
+        <c:axId val="-2145787112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,7 +2218,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2050896360"/>
+        <c:crossAx val="-2145790184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2266,11 +2444,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2055141832"/>
-        <c:axId val="-2055051320"/>
+        <c:axId val="-2145754280"/>
+        <c:axId val="-2145751208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2055141832"/>
+        <c:axId val="-2145754280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2280,7 +2458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2055051320"/>
+        <c:crossAx val="-2145751208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2288,7 +2466,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2055051320"/>
+        <c:axId val="-2145751208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2299,7 +2477,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2055141832"/>
+        <c:crossAx val="-2145754280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2525,11 +2703,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2055042248"/>
-        <c:axId val="-2054882744"/>
+        <c:axId val="-2145720040"/>
+        <c:axId val="-2145716968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2055042248"/>
+        <c:axId val="-2145720040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2539,7 +2717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054882744"/>
+        <c:crossAx val="-2145716968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2547,7 +2725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2054882744"/>
+        <c:axId val="-2145716968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,7 +2736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2055042248"/>
+        <c:crossAx val="-2145720040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2784,11 +2962,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2054849208"/>
-        <c:axId val="-2054832088"/>
+        <c:axId val="-2145685384"/>
+        <c:axId val="-2145682312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2054849208"/>
+        <c:axId val="-2145685384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2976,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054832088"/>
+        <c:crossAx val="-2145682312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2806,7 +2984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2054832088"/>
+        <c:axId val="-2145682312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2817,7 +2995,701 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2054849208"/>
+        <c:crossAx val="-2145685384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400">
+                <a:latin typeface="Helvetica"/>
+                <a:cs typeface="Helvetica"/>
+              </a:rPr>
+              <a:t>WordPress</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>10 sec</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$28:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$28:$F$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-60.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-65.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-68.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-46.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>10 min</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$28:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$28:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-104.49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-114.51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-123.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-120.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>1 hr</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$28:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$28:$N$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-60.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-65.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-67.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-62.90000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 hr</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$28:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$28:$R$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-104.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-112.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-114.38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.85999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2128044056"/>
+        <c:axId val="-2128040968"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2128044056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="28575" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1">
+                <a:latin typeface="Helvetica"/>
+                <a:cs typeface="Helvetica"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2128040968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2128040968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="28575" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1">
+                <a:latin typeface="Helvetica"/>
+                <a:cs typeface="Helvetica"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2128044056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="1">
+                <a:latin typeface="Helvetica"/>
+                <a:cs typeface="Helvetica"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="1">
+                <a:latin typeface="Helvetica"/>
+                <a:cs typeface="Helvetica"/>
+              </a:rPr>
+              <a:t>Couchbase</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>10 sec</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$11:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>50.00000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.00000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.00000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.00000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>10 min</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$11:$J$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-338.2500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-430.0000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-730.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-670.0000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>1 hr</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$11:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-412.49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-669.9999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-599.9999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-290.0000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>10 hr</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$11:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-293.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-299.9999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-240.0000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-30.00000000000025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2124688328"/>
+        <c:axId val="-2124749736"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2124688328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="28575" cmpd="sng">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1">
+                <a:latin typeface="Helvetica"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2124749736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2124749736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="28575" cmpd="sng"/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1">
+                <a:latin typeface="Helvetica"/>
+                <a:cs typeface="Helvetica"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2124688328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3027,6 +3899,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3393,12 +4330,12 @@
         <v>10</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="58" t="s">
+      <c r="O4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="59"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="64"/>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="6"/>
@@ -3438,12 +4375,12 @@
     <row r="6" spans="1:18">
       <c r="A6" s="6"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
       <c r="G6" s="44"/>
       <c r="H6" s="8"/>
       <c r="I6" t="s">
@@ -3481,14 +4418,14 @@
     <row r="7" spans="1:18">
       <c r="A7" s="6"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="61" t="s">
+      <c r="D7" s="65"/>
+      <c r="E7" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="62"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="14" t="s">
         <v>30</v>
       </c>
@@ -3780,12 +4717,12 @@
       <c r="G18" s="21"/>
       <c r="H18" s="22"/>
       <c r="N18" s="40"/>
-      <c r="O18" s="53" t="s">
+      <c r="O18" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="54"/>
+      <c r="P18" s="58"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="59"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="23"/>
@@ -3813,12 +4750,12 @@
     <row r="20" spans="1:18">
       <c r="A20" s="23"/>
       <c r="B20" s="26"/>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="54"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
       <c r="G20" s="24"/>
       <c r="H20" s="25"/>
       <c r="I20" t="s">
@@ -3847,14 +4784,14 @@
     <row r="21" spans="1:18">
       <c r="A21" s="23"/>
       <c r="B21" s="27"/>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56" t="s">
+      <c r="D21" s="60"/>
+      <c r="E21" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="57"/>
+      <c r="F21" s="62"/>
       <c r="G21" s="28" t="s">
         <v>30</v>
       </c>
@@ -4219,8 +5156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="I5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AF21" sqref="AF21"/>
+    <sheetView showRuler="0" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4261,18 +5198,18 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="51"/>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="G5" s="63" t="s">
+      <c r="D5" s="68"/>
+      <c r="G5" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="63"/>
-      <c r="K5" s="63" t="s">
+      <c r="H5" s="68"/>
+      <c r="K5" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="63"/>
+      <c r="L5" s="68"/>
       <c r="O5" s="51"/>
     </row>
     <row r="6" spans="1:15">
@@ -4320,45 +5257,45 @@
       <c r="B7" s="50">
         <v>0.5</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="54">
         <v>259.07</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="54">
         <v>258.98</v>
       </c>
-      <c r="E7" s="66">
+      <c r="E7" s="55">
         <f t="shared" ref="E7:E10" si="0">D7-C7</f>
         <v>-8.9999999999974989E-2</v>
       </c>
-      <c r="F7" s="68">
+      <c r="F7" s="57">
         <f>E7/C7</f>
         <v>-3.4739645655604658E-4</v>
       </c>
-      <c r="G7" s="65">
+      <c r="G7" s="54">
         <v>256.10000000000002</v>
       </c>
-      <c r="H7" s="65">
+      <c r="H7" s="54">
         <v>257.69</v>
       </c>
-      <c r="I7" s="66">
+      <c r="I7" s="55">
         <f>H7-G7</f>
         <v>1.589999999999975</v>
       </c>
-      <c r="J7" s="68">
+      <c r="J7" s="57">
         <f>I7/G7</f>
         <v>6.2085122998827603E-3</v>
       </c>
-      <c r="K7" s="65">
+      <c r="K7" s="54">
         <v>254.03</v>
       </c>
-      <c r="L7" s="65">
+      <c r="L7" s="54">
         <v>254.72</v>
       </c>
-      <c r="M7" s="66">
+      <c r="M7" s="55">
         <f>L7-K7</f>
         <v>0.68999999999999773</v>
       </c>
-      <c r="N7" s="68">
+      <c r="N7" s="57">
         <f>M7/K7</f>
         <v>2.7162146203204254E-3</v>
       </c>
@@ -4369,45 +5306,45 @@
       <c r="B8" s="50">
         <v>0.75</v>
       </c>
-      <c r="C8" s="65">
+      <c r="C8" s="54">
         <v>260.69</v>
       </c>
-      <c r="D8" s="65">
+      <c r="D8" s="54">
         <v>260.60000000000002</v>
       </c>
-      <c r="E8" s="66">
+      <c r="E8" s="55">
         <f t="shared" si="0"/>
         <v>-8.9999999999974989E-2</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="57">
         <f>E8/C8</f>
         <v>-3.452376385744562E-4</v>
       </c>
-      <c r="G8" s="65">
+      <c r="G8" s="54">
         <v>258.42</v>
       </c>
-      <c r="H8" s="65">
+      <c r="H8" s="54">
         <v>259.62</v>
       </c>
-      <c r="I8" s="66">
+      <c r="I8" s="55">
         <f t="shared" ref="I8:I10" si="1">H8-G8</f>
         <v>1.1999999999999886</v>
       </c>
-      <c r="J8" s="68">
+      <c r="J8" s="57">
         <f>I8/G8</f>
         <v>4.6436034362664982E-3</v>
       </c>
-      <c r="K8" s="65">
+      <c r="K8" s="54">
         <v>254.98</v>
       </c>
-      <c r="L8" s="65">
+      <c r="L8" s="54">
         <v>255.95</v>
       </c>
-      <c r="M8" s="66">
+      <c r="M8" s="55">
         <f t="shared" ref="M8:M10" si="2">L8-K8</f>
         <v>0.96999999999999886</v>
       </c>
-      <c r="N8" s="68">
+      <c r="N8" s="57">
         <f>M8/K8</f>
         <v>3.8042199388187265E-3</v>
       </c>
@@ -4418,45 +5355,45 @@
       <c r="B9" s="50">
         <v>0.9</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="54">
         <v>262.14999999999998</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="54">
         <v>262.19</v>
       </c>
-      <c r="E9" s="66">
+      <c r="E9" s="55">
         <f t="shared" si="0"/>
         <v>4.0000000000020464E-2</v>
       </c>
-      <c r="F9" s="68">
+      <c r="F9" s="57">
         <f>E9/C9</f>
         <v>1.525843982453575E-4</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="54">
         <v>260.54000000000002</v>
       </c>
-      <c r="H9" s="65">
+      <c r="H9" s="54">
         <v>261.33</v>
       </c>
-      <c r="I9" s="66">
+      <c r="I9" s="55">
         <f t="shared" si="1"/>
         <v>0.78999999999996362</v>
       </c>
-      <c r="J9" s="68">
+      <c r="J9" s="57">
         <f>I9/G9</f>
         <v>3.0321639671450204E-3</v>
       </c>
-      <c r="K9" s="65">
+      <c r="K9" s="54">
         <v>256.08</v>
       </c>
-      <c r="L9" s="65">
+      <c r="L9" s="54">
         <v>257.22000000000003</v>
       </c>
-      <c r="M9" s="66">
+      <c r="M9" s="55">
         <f t="shared" si="2"/>
         <v>1.1400000000000432</v>
       </c>
-      <c r="N9" s="68">
+      <c r="N9" s="57">
         <f>M9/K9</f>
         <v>4.4517338331773008E-3</v>
       </c>
@@ -4467,45 +5404,45 @@
       <c r="B10" s="50">
         <v>0.99</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="56">
         <v>265.04000000000002</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="54">
         <v>268.20999999999998</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="55">
         <f t="shared" si="0"/>
         <v>3.1699999999999591</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="57">
         <f>E10/C10</f>
         <v>1.1960458798671744E-2</v>
       </c>
-      <c r="G10" s="67">
+      <c r="G10" s="56">
         <v>263.44</v>
       </c>
-      <c r="H10" s="65">
+      <c r="H10" s="54">
         <v>265.51</v>
       </c>
-      <c r="I10" s="66">
+      <c r="I10" s="55">
         <f t="shared" si="1"/>
         <v>2.0699999999999932</v>
       </c>
-      <c r="J10" s="68">
+      <c r="J10" s="57">
         <f>I10/G10</f>
         <v>7.8575766778013704E-3</v>
       </c>
-      <c r="K10" s="67">
+      <c r="K10" s="56">
         <v>259.37</v>
       </c>
-      <c r="L10" s="65">
+      <c r="L10" s="54">
         <v>261.10000000000002</v>
       </c>
-      <c r="M10" s="66">
+      <c r="M10" s="55">
         <f t="shared" si="2"/>
         <v>1.7300000000000182</v>
       </c>
-      <c r="N10" s="68">
+      <c r="N10" s="57">
         <f>M10/K10</f>
         <v>6.6700080965416903E-3</v>
       </c>
@@ -4609,10 +5546,10 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="40"/>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="64"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="40"/>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
@@ -4628,18 +5565,18 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="40"/>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="63"/>
-      <c r="G22" s="63" t="s">
+      <c r="D22" s="68"/>
+      <c r="G22" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="63"/>
-      <c r="K22" s="63" t="s">
+      <c r="H22" s="68"/>
+      <c r="K22" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="63"/>
+      <c r="L22" s="68"/>
       <c r="O22" s="40"/>
     </row>
     <row r="23" spans="1:15">
@@ -4693,11 +5630,11 @@
       <c r="D24" s="45">
         <v>305.12</v>
       </c>
-      <c r="E24" s="66">
+      <c r="E24" s="55">
         <f t="shared" ref="E24:E27" si="3">D24-C24</f>
         <v>9.3600000000000136</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="57">
         <f>E24/C24</f>
         <v>3.164728157965923E-2</v>
       </c>
@@ -4707,11 +5644,11 @@
       <c r="H24" s="45">
         <v>306.22000000000003</v>
       </c>
-      <c r="I24" s="66">
+      <c r="I24" s="55">
         <f>H24-G24</f>
         <v>12.700000000000045</v>
       </c>
-      <c r="J24" s="68">
+      <c r="J24" s="57">
         <f>I24/G24</f>
         <v>4.3267920414281978E-2</v>
       </c>
@@ -4721,11 +5658,11 @@
       <c r="L24" s="45">
         <v>307.92</v>
       </c>
-      <c r="M24" s="66">
+      <c r="M24" s="55">
         <f>L24-K24</f>
         <v>10.140000000000043</v>
       </c>
-      <c r="N24" s="68">
+      <c r="N24" s="57">
         <f>M24/K24</f>
         <v>3.4051984686681594E-2</v>
       </c>
@@ -4742,11 +5679,11 @@
       <c r="D25" s="45">
         <v>318.2</v>
       </c>
-      <c r="E25" s="66">
+      <c r="E25" s="55">
         <f t="shared" si="3"/>
         <v>6.2899999999999636</v>
       </c>
-      <c r="F25" s="68">
+      <c r="F25" s="57">
         <f>E25/C25</f>
         <v>2.0166073546856348E-2</v>
       </c>
@@ -4756,11 +5693,11 @@
       <c r="H25" s="45">
         <v>317.33999999999997</v>
       </c>
-      <c r="I25" s="66">
+      <c r="I25" s="55">
         <f t="shared" ref="I25:I27" si="4">H25-G25</f>
         <v>12.339999999999975</v>
       </c>
-      <c r="J25" s="68">
+      <c r="J25" s="57">
         <f>I25/G25</f>
         <v>4.0459016393442543E-2</v>
       </c>
@@ -4770,11 +5707,11 @@
       <c r="L25" s="45">
         <v>318.95</v>
       </c>
-      <c r="M25" s="66">
+      <c r="M25" s="55">
         <f t="shared" ref="M25:M27" si="5">L25-K25</f>
         <v>13.349999999999966</v>
       </c>
-      <c r="N25" s="68">
+      <c r="N25" s="57">
         <f>M25/K25</f>
         <v>4.3684554973821878E-2</v>
       </c>
@@ -4791,11 +5728,11 @@
       <c r="D26" s="45">
         <v>327.47000000000003</v>
       </c>
-      <c r="E26" s="66">
+      <c r="E26" s="55">
         <f t="shared" si="3"/>
         <v>6.3500000000000227</v>
       </c>
-      <c r="F26" s="68">
+      <c r="F26" s="57">
         <f>E26/C26</f>
         <v>1.9774539113104207E-2</v>
       </c>
@@ -4805,11 +5742,11 @@
       <c r="H26" s="45">
         <v>326.23</v>
       </c>
-      <c r="I26" s="66">
+      <c r="I26" s="55">
         <f t="shared" si="4"/>
         <v>13.129999999999995</v>
       </c>
-      <c r="J26" s="68">
+      <c r="J26" s="57">
         <f>I26/G26</f>
         <v>4.1935483870967724E-2</v>
       </c>
@@ -4819,11 +5756,11 @@
       <c r="L26" s="45">
         <v>328.4</v>
       </c>
-      <c r="M26" s="66">
+      <c r="M26" s="55">
         <f t="shared" si="5"/>
         <v>16.21999999999997</v>
       </c>
-      <c r="N26" s="68">
+      <c r="N26" s="57">
         <f>M26/K26</f>
         <v>5.1957204177077235E-2</v>
       </c>
@@ -4840,11 +5777,11 @@
       <c r="D27" s="45">
         <v>341.44</v>
       </c>
-      <c r="E27" s="66">
+      <c r="E27" s="55">
         <f t="shared" si="3"/>
         <v>8.9599999999999795</v>
       </c>
-      <c r="F27" s="68">
+      <c r="F27" s="57">
         <f>E27/C27</f>
         <v>2.6948989412896952E-2</v>
       </c>
@@ -4854,11 +5791,11 @@
       <c r="H27" s="45">
         <v>340.11</v>
       </c>
-      <c r="I27" s="66">
+      <c r="I27" s="55">
         <f t="shared" si="4"/>
         <v>13.480000000000018</v>
       </c>
-      <c r="J27" s="68">
+      <c r="J27" s="57">
         <f>I27/G27</f>
         <v>4.1269938462480539E-2</v>
       </c>
@@ -4868,11 +5805,11 @@
       <c r="L27" s="45">
         <v>342.16</v>
       </c>
-      <c r="M27" s="66">
+      <c r="M27" s="55">
         <f t="shared" si="5"/>
         <v>16.54000000000002</v>
       </c>
-      <c r="N27" s="68">
+      <c r="N27" s="57">
         <f>M27/K27</f>
         <v>5.0795405687611386E-2</v>
       </c>
@@ -4997,4 +5934,1132 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:S36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:19">
+      <c r="B3" s="51"/>
+      <c r="C3" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="52"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+    </row>
+    <row r="4" spans="2:19">
+      <c r="B4" s="51"/>
+      <c r="D4" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="68"/>
+      <c r="H4" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="68"/>
+      <c r="L4" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" s="68"/>
+      <c r="P4" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" s="68"/>
+    </row>
+    <row r="5" spans="2:19">
+      <c r="B5" s="51"/>
+      <c r="D5" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P5" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="R5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19">
+      <c r="B6" s="51"/>
+      <c r="C6" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="54">
+        <v>1.29</v>
+      </c>
+      <c r="E6" s="54">
+        <v>1.34</v>
+      </c>
+      <c r="F6" s="55">
+        <f>(E6-D6)</f>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="G6" s="72">
+        <f>(F6/D6)</f>
+        <v>3.8759689922480654E-2</v>
+      </c>
+      <c r="H6" s="54">
+        <v>1.25</v>
+      </c>
+      <c r="I6" s="54">
+        <v>0.91174999999999995</v>
+      </c>
+      <c r="J6" s="55">
+        <f>(I6-H6)</f>
+        <v>-0.33825000000000005</v>
+      </c>
+      <c r="K6" s="72">
+        <f>(J6/H6)</f>
+        <v>-0.27060000000000006</v>
+      </c>
+      <c r="L6" s="54">
+        <v>1.32</v>
+      </c>
+      <c r="M6" s="54">
+        <v>0.90751000000000004</v>
+      </c>
+      <c r="N6" s="55">
+        <f>(M6-L6)</f>
+        <v>-0.41249000000000002</v>
+      </c>
+      <c r="O6" s="72">
+        <f>(N6/L6)</f>
+        <v>-0.31249242424242424</v>
+      </c>
+      <c r="P6" s="54">
+        <v>1.27</v>
+      </c>
+      <c r="Q6" s="54">
+        <v>0.97682999999999998</v>
+      </c>
+      <c r="R6" s="55">
+        <f>(Q6-P6)</f>
+        <v>-0.29317000000000004</v>
+      </c>
+      <c r="S6" s="72">
+        <f>(R6/P6)</f>
+        <v>-0.23084251968503941</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19">
+      <c r="B7" s="51"/>
+      <c r="C7" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="54">
+        <v>1.39</v>
+      </c>
+      <c r="E7" s="54">
+        <v>1.45</v>
+      </c>
+      <c r="F7" s="55">
+        <f t="shared" ref="F7:F9" si="0">(E7-D7)</f>
+        <v>6.0000000000000053E-2</v>
+      </c>
+      <c r="G7" s="72">
+        <f t="shared" ref="G7:G9" si="1">(F7/D7)</f>
+        <v>4.3165467625899324E-2</v>
+      </c>
+      <c r="H7" s="54">
+        <v>1.61</v>
+      </c>
+      <c r="I7" s="54">
+        <v>1.18</v>
+      </c>
+      <c r="J7" s="55">
+        <f t="shared" ref="J7:J9" si="2">(I7-H7)</f>
+        <v>-0.43000000000000016</v>
+      </c>
+      <c r="K7" s="72">
+        <f t="shared" ref="K7:K9" si="3">(J7/H7)</f>
+        <v>-0.26708074534161497</v>
+      </c>
+      <c r="L7" s="54">
+        <v>4.05</v>
+      </c>
+      <c r="M7" s="54">
+        <v>3.38</v>
+      </c>
+      <c r="N7" s="55">
+        <f t="shared" ref="N7:N9" si="4">(M7-L7)</f>
+        <v>-0.66999999999999993</v>
+      </c>
+      <c r="O7" s="72">
+        <f t="shared" ref="O7:O9" si="5">(N7/L7)</f>
+        <v>-0.16543209876543208</v>
+      </c>
+      <c r="P7" s="54">
+        <v>3.01</v>
+      </c>
+      <c r="Q7" s="54">
+        <v>2.71</v>
+      </c>
+      <c r="R7" s="55">
+        <f>(Q7-P7)</f>
+        <v>-0.29999999999999982</v>
+      </c>
+      <c r="S7" s="72">
+        <f t="shared" ref="S7:S9" si="6">(R7/P7)</f>
+        <v>-9.9667774086378683E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19">
+      <c r="B8" s="51"/>
+      <c r="C8" s="50">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="54">
+        <v>1.47</v>
+      </c>
+      <c r="E8" s="54">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="55">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="G8" s="72">
+        <f t="shared" si="1"/>
+        <v>2.0408163265306142E-2</v>
+      </c>
+      <c r="H8" s="54">
+        <v>3.25</v>
+      </c>
+      <c r="I8" s="54">
+        <v>2.52</v>
+      </c>
+      <c r="J8" s="55">
+        <f t="shared" si="2"/>
+        <v>-0.73</v>
+      </c>
+      <c r="K8" s="72">
+        <f t="shared" si="3"/>
+        <v>-0.22461538461538461</v>
+      </c>
+      <c r="L8" s="54">
+        <v>4.79</v>
+      </c>
+      <c r="M8" s="54">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="N8" s="55">
+        <f t="shared" si="4"/>
+        <v>-0.59999999999999964</v>
+      </c>
+      <c r="O8" s="72">
+        <f t="shared" si="5"/>
+        <v>-0.12526096033402914</v>
+      </c>
+      <c r="P8" s="54">
+        <v>5.59</v>
+      </c>
+      <c r="Q8" s="54">
+        <v>5.35</v>
+      </c>
+      <c r="R8" s="55">
+        <f t="shared" ref="R8:R9" si="7">(Q8-P8)</f>
+        <v>-0.24000000000000021</v>
+      </c>
+      <c r="S8" s="72">
+        <f t="shared" si="6"/>
+        <v>-4.2933810375670879E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19">
+      <c r="B9" s="51"/>
+      <c r="C9" s="50">
+        <v>0.99</v>
+      </c>
+      <c r="D9" s="56">
+        <v>1.52</v>
+      </c>
+      <c r="E9" s="54">
+        <v>1.6</v>
+      </c>
+      <c r="F9" s="55">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="G9" s="72">
+        <f t="shared" si="1"/>
+        <v>5.2631578947368467E-2</v>
+      </c>
+      <c r="H9" s="56">
+        <v>4.24</v>
+      </c>
+      <c r="I9" s="54">
+        <v>3.57</v>
+      </c>
+      <c r="J9" s="55">
+        <f t="shared" si="2"/>
+        <v>-0.67000000000000037</v>
+      </c>
+      <c r="K9" s="72">
+        <f t="shared" si="3"/>
+        <v>-0.15801886792452838</v>
+      </c>
+      <c r="L9" s="56">
+        <v>5.75</v>
+      </c>
+      <c r="M9" s="54">
+        <v>5.46</v>
+      </c>
+      <c r="N9" s="55">
+        <f t="shared" si="4"/>
+        <v>-0.29000000000000004</v>
+      </c>
+      <c r="O9" s="72">
+        <f t="shared" si="5"/>
+        <v>-5.0434782608695661E-2</v>
+      </c>
+      <c r="P9" s="56">
+        <v>7.44</v>
+      </c>
+      <c r="Q9" s="54">
+        <v>7.41</v>
+      </c>
+      <c r="R9" s="55">
+        <f t="shared" si="7"/>
+        <v>-3.0000000000000249E-2</v>
+      </c>
+      <c r="S9" s="72">
+        <f t="shared" si="6"/>
+        <v>-4.0322580645161619E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19">
+      <c r="B10" s="51"/>
+    </row>
+    <row r="11" spans="2:19">
+      <c r="B11" s="51"/>
+      <c r="C11" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="69">
+        <f>D6*1000</f>
+        <v>1290</v>
+      </c>
+      <c r="E11" s="69">
+        <f t="shared" ref="E11:R11" si="8">E6*1000</f>
+        <v>1340</v>
+      </c>
+      <c r="F11" s="69">
+        <f t="shared" si="8"/>
+        <v>50.000000000000043</v>
+      </c>
+      <c r="G11" s="72">
+        <f>(F11/D11)</f>
+        <v>3.8759689922480654E-2</v>
+      </c>
+      <c r="H11" s="69">
+        <f t="shared" si="8"/>
+        <v>1250</v>
+      </c>
+      <c r="I11" s="69">
+        <f t="shared" si="8"/>
+        <v>911.75</v>
+      </c>
+      <c r="J11" s="69">
+        <f t="shared" si="8"/>
+        <v>-338.25000000000006</v>
+      </c>
+      <c r="K11" s="72">
+        <f>(J11/H11)</f>
+        <v>-0.27060000000000006</v>
+      </c>
+      <c r="L11" s="69">
+        <f t="shared" si="8"/>
+        <v>1320</v>
+      </c>
+      <c r="M11" s="69">
+        <f t="shared" si="8"/>
+        <v>907.51</v>
+      </c>
+      <c r="N11" s="69">
+        <f t="shared" si="8"/>
+        <v>-412.49</v>
+      </c>
+      <c r="O11" s="72">
+        <f>(N11/L11)</f>
+        <v>-0.31249242424242424</v>
+      </c>
+      <c r="P11" s="69">
+        <f t="shared" si="8"/>
+        <v>1270</v>
+      </c>
+      <c r="Q11" s="69">
+        <f t="shared" si="8"/>
+        <v>976.82999999999993</v>
+      </c>
+      <c r="R11" s="69">
+        <f t="shared" si="8"/>
+        <v>-293.17</v>
+      </c>
+      <c r="S11" s="72">
+        <f>(R11/P11)</f>
+        <v>-0.23084251968503938</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19">
+      <c r="B12" s="51"/>
+      <c r="C12" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="69">
+        <f t="shared" ref="D12:R12" si="9">D7*1000</f>
+        <v>1390</v>
+      </c>
+      <c r="E12" s="69">
+        <f t="shared" si="9"/>
+        <v>1450</v>
+      </c>
+      <c r="F12" s="69">
+        <f t="shared" si="9"/>
+        <v>60.000000000000057</v>
+      </c>
+      <c r="G12" s="72">
+        <f t="shared" ref="G12:G14" si="10">(F12/D12)</f>
+        <v>4.3165467625899324E-2</v>
+      </c>
+      <c r="H12" s="69">
+        <f t="shared" si="9"/>
+        <v>1610</v>
+      </c>
+      <c r="I12" s="69">
+        <f t="shared" si="9"/>
+        <v>1180</v>
+      </c>
+      <c r="J12" s="69">
+        <f t="shared" si="9"/>
+        <v>-430.00000000000017</v>
+      </c>
+      <c r="K12" s="72">
+        <f t="shared" ref="K12:K14" si="11">(J12/H12)</f>
+        <v>-0.26708074534161502</v>
+      </c>
+      <c r="L12" s="69">
+        <f t="shared" si="9"/>
+        <v>4050</v>
+      </c>
+      <c r="M12" s="69">
+        <f t="shared" si="9"/>
+        <v>3380</v>
+      </c>
+      <c r="N12" s="69">
+        <f t="shared" si="9"/>
+        <v>-669.99999999999989</v>
+      </c>
+      <c r="O12" s="72">
+        <f t="shared" ref="O12:O14" si="12">(N12/L12)</f>
+        <v>-0.16543209876543208</v>
+      </c>
+      <c r="P12" s="69">
+        <f t="shared" si="9"/>
+        <v>3010</v>
+      </c>
+      <c r="Q12" s="69">
+        <f t="shared" si="9"/>
+        <v>2710</v>
+      </c>
+      <c r="R12" s="69">
+        <f t="shared" si="9"/>
+        <v>-299.99999999999983</v>
+      </c>
+      <c r="S12" s="72">
+        <f t="shared" ref="S12:S14" si="13">(R12/P12)</f>
+        <v>-9.9667774086378683E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19">
+      <c r="B13" s="51"/>
+      <c r="C13" s="50">
+        <v>0.9</v>
+      </c>
+      <c r="D13" s="69">
+        <f t="shared" ref="D13:R13" si="14">D8*1000</f>
+        <v>1470</v>
+      </c>
+      <c r="E13" s="69">
+        <f t="shared" si="14"/>
+        <v>1500</v>
+      </c>
+      <c r="F13" s="69">
+        <f t="shared" si="14"/>
+        <v>30.000000000000028</v>
+      </c>
+      <c r="G13" s="72">
+        <f t="shared" si="10"/>
+        <v>2.0408163265306142E-2</v>
+      </c>
+      <c r="H13" s="69">
+        <f t="shared" si="14"/>
+        <v>3250</v>
+      </c>
+      <c r="I13" s="69">
+        <f t="shared" si="14"/>
+        <v>2520</v>
+      </c>
+      <c r="J13" s="69">
+        <f t="shared" si="14"/>
+        <v>-730</v>
+      </c>
+      <c r="K13" s="72">
+        <f t="shared" si="11"/>
+        <v>-0.22461538461538461</v>
+      </c>
+      <c r="L13" s="69">
+        <f t="shared" si="14"/>
+        <v>4790</v>
+      </c>
+      <c r="M13" s="69">
+        <f t="shared" si="14"/>
+        <v>4190</v>
+      </c>
+      <c r="N13" s="69">
+        <f t="shared" si="14"/>
+        <v>-599.99999999999966</v>
+      </c>
+      <c r="O13" s="72">
+        <f t="shared" si="12"/>
+        <v>-0.12526096033402917</v>
+      </c>
+      <c r="P13" s="69">
+        <f t="shared" si="14"/>
+        <v>5590</v>
+      </c>
+      <c r="Q13" s="69">
+        <f t="shared" si="14"/>
+        <v>5350</v>
+      </c>
+      <c r="R13" s="69">
+        <f t="shared" si="14"/>
+        <v>-240.00000000000023</v>
+      </c>
+      <c r="S13" s="72">
+        <f t="shared" si="13"/>
+        <v>-4.2933810375670879E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19">
+      <c r="B14" s="51"/>
+      <c r="C14" s="50">
+        <v>0.99</v>
+      </c>
+      <c r="D14" s="69">
+        <f t="shared" ref="D14:R14" si="15">D9*1000</f>
+        <v>1520</v>
+      </c>
+      <c r="E14" s="69">
+        <f t="shared" si="15"/>
+        <v>1600</v>
+      </c>
+      <c r="F14" s="69">
+        <f t="shared" si="15"/>
+        <v>80.000000000000071</v>
+      </c>
+      <c r="G14" s="72">
+        <f t="shared" si="10"/>
+        <v>5.2631578947368467E-2</v>
+      </c>
+      <c r="H14" s="69">
+        <f t="shared" si="15"/>
+        <v>4240</v>
+      </c>
+      <c r="I14" s="69">
+        <f t="shared" si="15"/>
+        <v>3570</v>
+      </c>
+      <c r="J14" s="69">
+        <f t="shared" si="15"/>
+        <v>-670.00000000000034</v>
+      </c>
+      <c r="K14" s="72">
+        <f t="shared" si="11"/>
+        <v>-0.15801886792452838</v>
+      </c>
+      <c r="L14" s="69">
+        <f t="shared" si="15"/>
+        <v>5750</v>
+      </c>
+      <c r="M14" s="69">
+        <f t="shared" si="15"/>
+        <v>5460</v>
+      </c>
+      <c r="N14" s="69">
+        <f t="shared" si="15"/>
+        <v>-290.00000000000006</v>
+      </c>
+      <c r="O14" s="72">
+        <f t="shared" si="12"/>
+        <v>-5.0434782608695661E-2</v>
+      </c>
+      <c r="P14" s="69">
+        <f t="shared" si="15"/>
+        <v>7440</v>
+      </c>
+      <c r="Q14" s="69">
+        <f t="shared" si="15"/>
+        <v>7410</v>
+      </c>
+      <c r="R14" s="69">
+        <f t="shared" si="15"/>
+        <v>-30.000000000000249</v>
+      </c>
+      <c r="S14" s="72">
+        <f t="shared" si="13"/>
+        <v>-4.0322580645161627E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19">
+      <c r="B15" s="51"/>
+    </row>
+    <row r="16" spans="2:19">
+      <c r="B16" s="51"/>
+      <c r="C16" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="45"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="45"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="45"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="45"/>
+    </row>
+    <row r="17" spans="2:19">
+      <c r="B17" s="51"/>
+      <c r="C17" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+    </row>
+    <row r="18" spans="2:19">
+      <c r="B18" s="51"/>
+      <c r="C18" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="49"/>
+      <c r="E18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="P18" s="45"/>
+    </row>
+    <row r="19" spans="2:19">
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+    </row>
+    <row r="25" spans="2:19">
+      <c r="B25" s="40"/>
+      <c r="C25" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="53"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+    </row>
+    <row r="26" spans="2:19">
+      <c r="B26" s="40"/>
+      <c r="D26" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="68"/>
+      <c r="H26" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="68"/>
+      <c r="L26" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="M26" s="68"/>
+      <c r="P26" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q26" s="68"/>
+    </row>
+    <row r="27" spans="2:19">
+      <c r="B27" s="40"/>
+      <c r="D27" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="J27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="M27" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="N27" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" t="s">
+        <v>72</v>
+      </c>
+      <c r="P27" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="R27" t="s">
+        <v>30</v>
+      </c>
+      <c r="S27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19">
+      <c r="B28" s="40"/>
+      <c r="C28" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="69">
+        <v>120.67</v>
+      </c>
+      <c r="E28" s="69">
+        <v>60.45</v>
+      </c>
+      <c r="F28" s="70">
+        <f>(E28-D28)</f>
+        <v>-60.22</v>
+      </c>
+      <c r="G28" s="72">
+        <f>(F28/D28)</f>
+        <v>-0.49904698765227479</v>
+      </c>
+      <c r="H28" s="69">
+        <v>169.48</v>
+      </c>
+      <c r="I28" s="69">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="J28" s="70">
+        <f>(I28-H28)</f>
+        <v>-104.49</v>
+      </c>
+      <c r="K28" s="72">
+        <f>(J28/H28)</f>
+        <v>-0.6165329242388482</v>
+      </c>
+      <c r="L28" s="69">
+        <v>126.75</v>
+      </c>
+      <c r="M28" s="70">
+        <v>66.63</v>
+      </c>
+      <c r="N28" s="70">
+        <f>(M28-L28)</f>
+        <v>-60.120000000000005</v>
+      </c>
+      <c r="O28" s="72">
+        <f>(N28/L28)</f>
+        <v>-0.47431952662721899</v>
+      </c>
+      <c r="P28" s="70">
+        <v>169.06</v>
+      </c>
+      <c r="Q28" s="70">
+        <v>64.37</v>
+      </c>
+      <c r="R28" s="70">
+        <f>(Q28-P28)</f>
+        <v>-104.69</v>
+      </c>
+      <c r="S28" s="72">
+        <f>(R28/P28)</f>
+        <v>-0.6192476044008044</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19">
+      <c r="B29" s="40"/>
+      <c r="C29" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="D29" s="69">
+        <v>135.22999999999999</v>
+      </c>
+      <c r="E29" s="69">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="F29" s="70">
+        <f t="shared" ref="F29:F31" si="16">(E29-D29)</f>
+        <v>-65.88</v>
+      </c>
+      <c r="G29" s="72">
+        <f t="shared" ref="G29:G31" si="17">(F29/D29)</f>
+        <v>-0.48717000665532795</v>
+      </c>
+      <c r="H29" s="69">
+        <v>190.09</v>
+      </c>
+      <c r="I29" s="69">
+        <v>75.58</v>
+      </c>
+      <c r="J29" s="70">
+        <f t="shared" ref="J29:J31" si="18">(I29-H29)</f>
+        <v>-114.51</v>
+      </c>
+      <c r="K29" s="72">
+        <f t="shared" ref="K29:K31" si="19">(J29/H29)</f>
+        <v>-0.60239886369614393</v>
+      </c>
+      <c r="L29" s="69">
+        <v>142.4</v>
+      </c>
+      <c r="M29" s="70">
+        <v>77.39</v>
+      </c>
+      <c r="N29" s="70">
+        <f t="shared" ref="N29:N31" si="20">(M29-L29)</f>
+        <v>-65.010000000000005</v>
+      </c>
+      <c r="O29" s="72">
+        <f t="shared" ref="O29:O31" si="21">(N29/L29)</f>
+        <v>-0.45653089887640452</v>
+      </c>
+      <c r="P29" s="70">
+        <v>188.47</v>
+      </c>
+      <c r="Q29" s="70">
+        <v>75.94</v>
+      </c>
+      <c r="R29" s="70">
+        <f t="shared" ref="R29:R31" si="22">(Q29-P29)</f>
+        <v>-112.53</v>
+      </c>
+      <c r="S29" s="72">
+        <f t="shared" ref="S29:S31" si="23">(R29/P29)</f>
+        <v>-0.5970711519074654</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19">
+      <c r="B30" s="40"/>
+      <c r="C30" s="50">
+        <v>0.9</v>
+      </c>
+      <c r="D30" s="69">
+        <v>146.34</v>
+      </c>
+      <c r="E30" s="69">
+        <v>78.23</v>
+      </c>
+      <c r="F30" s="70">
+        <f t="shared" si="16"/>
+        <v>-68.11</v>
+      </c>
+      <c r="G30" s="72">
+        <f t="shared" si="17"/>
+        <v>-0.46542298756320893</v>
+      </c>
+      <c r="H30" s="69">
+        <v>209.47</v>
+      </c>
+      <c r="I30" s="69">
+        <v>86.27</v>
+      </c>
+      <c r="J30" s="70">
+        <f t="shared" si="18"/>
+        <v>-123.2</v>
+      </c>
+      <c r="K30" s="72">
+        <f t="shared" si="19"/>
+        <v>-0.58815104788275174</v>
+      </c>
+      <c r="L30" s="69">
+        <v>156.52000000000001</v>
+      </c>
+      <c r="M30" s="70">
+        <v>88.72</v>
+      </c>
+      <c r="N30" s="70">
+        <f t="shared" si="20"/>
+        <v>-67.800000000000011</v>
+      </c>
+      <c r="O30" s="72">
+        <f t="shared" si="21"/>
+        <v>-0.43317147968310765</v>
+      </c>
+      <c r="P30" s="70">
+        <v>206.23</v>
+      </c>
+      <c r="Q30" s="70">
+        <v>91.85</v>
+      </c>
+      <c r="R30" s="70">
+        <f t="shared" si="22"/>
+        <v>-114.38</v>
+      </c>
+      <c r="S30" s="72">
+        <f t="shared" si="23"/>
+        <v>-0.554623478640353</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19">
+      <c r="B31" s="40"/>
+      <c r="C31" s="50">
+        <v>0.99</v>
+      </c>
+      <c r="D31" s="71">
+        <v>170.16</v>
+      </c>
+      <c r="E31" s="69">
+        <v>123.46</v>
+      </c>
+      <c r="F31" s="70">
+        <f t="shared" si="16"/>
+        <v>-46.7</v>
+      </c>
+      <c r="G31" s="72">
+        <f t="shared" si="17"/>
+        <v>-0.27444757874941234</v>
+      </c>
+      <c r="H31" s="71">
+        <v>257.86</v>
+      </c>
+      <c r="I31" s="69">
+        <v>137.47</v>
+      </c>
+      <c r="J31" s="70">
+        <f t="shared" si="18"/>
+        <v>-120.39000000000001</v>
+      </c>
+      <c r="K31" s="72">
+        <f t="shared" si="19"/>
+        <v>-0.46688125339331421</v>
+      </c>
+      <c r="L31" s="71">
+        <v>183.3</v>
+      </c>
+      <c r="M31" s="70">
+        <v>120.4</v>
+      </c>
+      <c r="N31" s="70">
+        <f t="shared" si="20"/>
+        <v>-62.900000000000006</v>
+      </c>
+      <c r="O31" s="72">
+        <f t="shared" si="21"/>
+        <v>-0.34315330060010912</v>
+      </c>
+      <c r="P31" s="70">
+        <v>238.47</v>
+      </c>
+      <c r="Q31" s="70">
+        <v>277.33</v>
+      </c>
+      <c r="R31" s="70">
+        <f t="shared" si="22"/>
+        <v>38.859999999999985</v>
+      </c>
+      <c r="S31" s="72">
+        <f t="shared" si="23"/>
+        <v>0.16295550803036016</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19">
+      <c r="B32" s="40"/>
+    </row>
+    <row r="33" spans="2:17">
+      <c r="B33" s="40"/>
+      <c r="C33" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="48"/>
+      <c r="E33" s="45"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="45"/>
+      <c r="L33" s="48"/>
+      <c r="M33" s="45"/>
+      <c r="P33" s="48"/>
+      <c r="Q33" s="45"/>
+    </row>
+    <row r="34" spans="2:17">
+      <c r="B34" s="40"/>
+      <c r="C34" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+    </row>
+    <row r="35" spans="2:17">
+      <c r="B35" s="40"/>
+      <c r="C35" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="49"/>
+      <c r="E35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="P35" s="45"/>
+    </row>
+    <row r="36" spans="2:17">
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="L26:M26"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F28:F31 J28:J31 N28:N31 R28:R31 R11:R14 N11:N14 J11:J14 F11:F14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>